<commit_message>
added feature for checking with valid errors
</commit_message>
<xml_diff>
--- a/mismatches.xlsx
+++ b/mismatches.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>left_only</t>
+          <t>right_only</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -485,7 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>right_only</t>
+          <t>left_only</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>